<commit_message>
feat:sound and mushroom hight
</commit_message>
<xml_diff>
--- a/Excels/Sound_音效表.xlsx
+++ b/Excels/Sound_音效表.xlsx
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5666666666667" defaultRowHeight="16.5"/>
@@ -1692,19 +1692,19 @@
         <v>1</v>
       </c>
       <c r="E12" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="4">
         <v>200</v>
       </c>
       <c r="I12" s="4">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="J12" s="4"/>
     </row>
@@ -1743,7 +1743,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="4">
-        <v>202244</v>
+        <v>201870</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>34</v>
@@ -1758,13 +1758,13 @@
         <v>1</v>
       </c>
       <c r="G14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="4">
         <v>200</v>
       </c>
       <c r="I14" s="4">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>35</v>
@@ -1790,13 +1790,13 @@
         <v>1</v>
       </c>
       <c r="G15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4">
         <v>200</v>
       </c>
       <c r="I15" s="4">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="J15" s="4"/>
     </row>
@@ -1820,13 +1820,13 @@
         <v>1</v>
       </c>
       <c r="G16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="4">
         <v>200</v>
       </c>
       <c r="I16" s="4">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="J16" s="4"/>
     </row>
@@ -1850,13 +1850,13 @@
         <v>1</v>
       </c>
       <c r="G17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="4">
         <v>200</v>
       </c>
       <c r="I17" s="4">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="J17" s="4"/>
     </row>

</xml_diff>

<commit_message>
feat:light dark tips and sound excel
</commit_message>
<xml_diff>
--- a/Excels/Sound_音效表.xlsx
+++ b/Excels/Sound_音效表.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>int</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>跑酷：结算音效</t>
+  </si>
+  <si>
+    <t>主世界bgm1</t>
+  </si>
+  <si>
+    <t>主世界bgm2</t>
   </si>
 </sst>
 </file>
@@ -808,7 +814,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -818,6 +824,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1353,10 +1362,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5666666666667" defaultRowHeight="16.5"/>
@@ -2223,6 +2232,106 @@
         <v>600</v>
       </c>
       <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="5">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>200</v>
+      </c>
+      <c r="I30" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="5">
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>200</v>
+      </c>
+      <c r="I31" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="5"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="5"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="5"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>